<commit_message>
Update am 22.10.2018 um 14:03 Uhr
</commit_message>
<xml_diff>
--- a/Kommunikationsprotokolle.xlsx
+++ b/Kommunikationsprotokolle.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B52CB4A-33F5-45C8-871A-E3FB8E9BF558}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="11025" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SM" sheetId="3" r:id="rId1"/>
@@ -12,8 +13,8 @@
     <sheet name="SummenTelegramm" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="117">
   <si>
     <t>Status</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -469,12 +470,44 @@
     <t>AP-Tabelle</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>105...De_cacu ask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>103...Handshake_ask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>106...De_cacu_ans</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>107...Sum_De_cacu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>104...Handshake_ans</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -533,6 +566,12 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -548,7 +587,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="49">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -1152,11 +1191,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1275,24 +1373,12 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1300,9 +1386,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1344,6 +1427,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1377,61 +1493,85 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1440,91 +1580,88 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1799,43 +1936,43 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.58203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="2.58203125" style="1" customWidth="1"/>
-    <col min="3" max="10" width="15.58203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2.625" style="1" customWidth="1"/>
+    <col min="3" max="10" width="15.625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="27" customHeight="1" thickBot="1">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-    </row>
-    <row r="2" spans="1:10" ht="14.25" customHeight="1" thickBot="1">
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+    </row>
+    <row r="2" spans="1:10" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -1847,14 +1984,14 @@
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:10" ht="14.5" thickBot="1">
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="56" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -1876,8 +2013,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="70" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="76" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="3">
@@ -1890,8 +2027,8 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="70"/>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="76"/>
       <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1902,15 +2039,15 @@
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
     </row>
-    <row r="6" spans="1:10" ht="14.5" thickBot="1">
-      <c r="A6" s="70"/>
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="76"/>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:10" ht="14.5" thickBot="1">
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="C7" s="22" t="s">
         <v>106</v>
@@ -1923,14 +2060,14 @@
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
     </row>
-    <row r="8" spans="1:10" ht="14.5" thickBot="1">
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H8" s="9"/>
     </row>
-    <row r="9" spans="1:10" ht="14.5" thickBot="1">
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="61" t="s">
+      <c r="D9" s="56" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -1949,11 +2086,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
-      <c r="D10" s="66" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D10" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="68"/>
+      <c r="E10" s="74"/>
       <c r="F10" s="2" t="s">
         <v>1</v>
       </c>
@@ -1961,9 +2098,9 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:10">
-      <c r="D11" s="67"/>
-      <c r="E11" s="68"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D11" s="73"/>
+      <c r="E11" s="74"/>
       <c r="F11" s="2" t="s">
         <v>2</v>
       </c>
@@ -1971,7 +2108,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="14.5" thickBot="1">
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -1983,21 +2120,21 @@
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" spans="1:10" ht="14.5" thickBot="1">
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
     </row>
-    <row r="14" spans="1:10" ht="14.5" thickBot="1">
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="61" t="s">
+      <c r="D14" s="56" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -2007,33 +2144,33 @@
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="14" customHeight="1">
-      <c r="A15" s="70" t="s">
+    <row r="15" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="76" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="3">
         <v>1</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="62"/>
-    </row>
-    <row r="16" spans="1:10" ht="14" customHeight="1">
-      <c r="A16" s="70"/>
+      <c r="F15" s="57"/>
+    </row>
+    <row r="16" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="76"/>
       <c r="D16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="62"/>
-    </row>
-    <row r="17" spans="1:11" ht="14" customHeight="1" thickBot="1">
-      <c r="A17" s="70"/>
-    </row>
-    <row r="18" spans="1:11" ht="14" customHeight="1" thickBot="1">
-      <c r="A18" s="60"/>
+      <c r="F16" s="57"/>
+    </row>
+    <row r="17" spans="1:11" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="76"/>
+    </row>
+    <row r="18" spans="1:11" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="55"/>
       <c r="C18" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="56" t="s">
         <v>1</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -2049,7 +2186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D19" s="11">
         <v>1</v>
       </c>
@@ -2058,7 +2195,7 @@
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D20" s="11">
         <v>2</v>
       </c>
@@ -2067,7 +2204,7 @@
       <c r="G20" s="20"/>
       <c r="H20" s="20"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D21" s="3">
         <v>3</v>
       </c>
@@ -2076,18 +2213,18 @@
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
     </row>
-    <row r="22" spans="1:11" ht="14.5" thickBot="1">
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
     </row>
-    <row r="23" spans="1:11" ht="14.5" thickBot="1">
+    <row r="23" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C23" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D23" s="61" t="s">
+      <c r="D23" s="56" t="s">
         <v>25</v>
       </c>
       <c r="E23" s="9"/>
@@ -2095,14 +2232,14 @@
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
     </row>
-    <row r="24" spans="1:11">
-      <c r="D24" s="62"/>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D24" s="57"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
     </row>
-    <row r="25" spans="1:11" ht="14.5" thickBot="1">
+    <row r="25" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -2114,7 +2251,7 @@
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
     </row>
-    <row r="26" spans="1:11" ht="14.5" thickBot="1">
+    <row r="26" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -2127,7 +2264,7 @@
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
     </row>
-    <row r="27" spans="1:11" ht="14.5" thickBot="1">
+    <row r="27" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
         <v>9</v>
       </c>
@@ -2145,8 +2282,8 @@
       <c r="J27" s="10"/>
       <c r="K27" s="9"/>
     </row>
-    <row r="28" spans="1:11" ht="14" customHeight="1">
-      <c r="A28" s="63" t="s">
+    <row r="28" spans="1:11" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="69" t="s">
         <v>2</v>
       </c>
       <c r="D28" s="16"/>
@@ -2156,8 +2293,8 @@
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
     </row>
-    <row r="29" spans="1:11" ht="14" customHeight="1" thickBot="1">
-      <c r="A29" s="64"/>
+    <row r="29" spans="1:11" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="70"/>
       <c r="D29" s="13"/>
       <c r="E29" s="8"/>
       <c r="H29" s="9"/>
@@ -2165,12 +2302,12 @@
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
     </row>
-    <row r="30" spans="1:11" ht="14" customHeight="1" thickBot="1">
-      <c r="A30" s="65"/>
+    <row r="30" spans="1:11" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="71"/>
       <c r="C30" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="D30" s="61" t="s">
+      <c r="D30" s="56" t="s">
         <v>25</v>
       </c>
       <c r="H30" s="9"/>
@@ -2178,22 +2315,22 @@
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
     </row>
-    <row r="31" spans="1:11" ht="14" customHeight="1">
-      <c r="A31" s="60"/>
+    <row r="31" spans="1:11" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="55"/>
       <c r="D31" s="3"/>
       <c r="H31" s="9"/>
       <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
     </row>
-    <row r="32" spans="1:11" ht="14" customHeight="1">
-      <c r="A32" s="60"/>
+    <row r="32" spans="1:11" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="55"/>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
     </row>
-    <row r="33" spans="8:11">
+    <row r="33" spans="8:11" x14ac:dyDescent="0.2">
       <c r="H33" s="9"/>
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
@@ -2215,66 +2352,66 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.58203125" style="6" customWidth="1"/>
-    <col min="3" max="6" width="15.58203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="9.58203125" style="5" customWidth="1"/>
+    <col min="1" max="2" width="9.625" style="6" customWidth="1"/>
+    <col min="3" max="6" width="15.625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="9.625" style="5" customWidth="1"/>
     <col min="8" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5" thickBot="1">
-      <c r="C1" s="71" t="s">
+    <row r="1" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="73"/>
-    </row>
-    <row r="2" spans="1:6" ht="14.5" thickBot="1">
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="79"/>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="17"/>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="53" t="s">
+      <c r="D2" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="52" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="21">
         <v>-1</v>
       </c>
       <c r="B3" s="17"/>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="F3" s="53" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="21">
         <v>0</v>
       </c>
@@ -2282,7 +2419,7 @@
       <c r="C4" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="55" t="s">
+      <c r="D4" s="50" t="s">
         <v>26</v>
       </c>
       <c r="E4" s="14" t="s">
@@ -2292,7 +2429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="21">
         <v>1</v>
       </c>
@@ -2300,7 +2437,7 @@
       <c r="C5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="55" t="s">
+      <c r="D5" s="50" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="14" t="s">
@@ -2310,7 +2447,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="21">
         <v>2</v>
       </c>
@@ -2318,7 +2455,7 @@
       <c r="C6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="55" t="s">
+      <c r="D6" s="50" t="s">
         <v>28</v>
       </c>
       <c r="E6" s="14" t="s">
@@ -2328,29 +2465,29 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.5" thickBot="1">
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
         <v>3</v>
       </c>
       <c r="B7" s="17"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="56" t="s">
+      <c r="C7" s="47"/>
+      <c r="D7" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="59"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="F7" s="54"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
     </row>
@@ -2365,99 +2502,107 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="H27" sqref="H27:I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="8.6640625" style="23"/>
-    <col min="3" max="3" width="8.6640625" style="23" customWidth="1"/>
-    <col min="4" max="7" width="8.6640625" style="23"/>
-    <col min="8" max="8" width="8.6640625" style="23" customWidth="1"/>
-    <col min="9" max="16384" width="8.6640625" style="23"/>
+    <col min="1" max="2" width="8.625" style="23"/>
+    <col min="3" max="3" width="8.625" style="23" customWidth="1"/>
+    <col min="4" max="7" width="8.625" style="23"/>
+    <col min="8" max="8" width="8.625" style="23" customWidth="1"/>
+    <col min="9" max="9" width="8.625" style="23"/>
+    <col min="10" max="10" width="2.625" style="23" customWidth="1"/>
+    <col min="11" max="11" width="8.625" style="23"/>
+    <col min="12" max="12" width="7.625" style="23" customWidth="1"/>
+    <col min="13" max="13" width="8.625" style="23"/>
+    <col min="14" max="14" width="7.625" style="23" customWidth="1"/>
+    <col min="15" max="15" width="8.625" style="23"/>
+    <col min="16" max="16" width="7.625" style="23" customWidth="1"/>
+    <col min="17" max="16384" width="8.625" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="28" thickBot="1">
-      <c r="A1" s="87" t="s">
+    <row r="1" spans="1:19" ht="28.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="89"/>
-    </row>
-    <row r="2" spans="1:19" ht="25" customHeight="1" thickBot="1">
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="82"/>
+    </row>
+    <row r="2" spans="1:19" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="103" t="s">
+      <c r="B2" s="87" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
-      <c r="H2" s="104"/>
-      <c r="I2" s="105"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="89"/>
       <c r="J2" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-    </row>
-    <row r="3" spans="1:19" ht="14.5" thickBot="1">
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+    </row>
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="90" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="108"/>
+      <c r="C3" s="91"/>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="92"/>
       <c r="J3" s="26" t="s">
         <v>6</v>
       </c>
       <c r="R3" s="27"/>
-      <c r="S3" s="25"/>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="S3" s="58"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="28"/>
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="100"/>
-      <c r="D4" s="101" t="s">
+      <c r="C4" s="84"/>
+      <c r="D4" s="85" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="102"/>
-      <c r="F4" s="99" t="s">
+      <c r="E4" s="86"/>
+      <c r="F4" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="100"/>
-      <c r="H4" s="101" t="s">
+      <c r="G4" s="84"/>
+      <c r="H4" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="102"/>
+      <c r="I4" s="86"/>
       <c r="J4" s="28"/>
       <c r="R4" s="27"/>
-      <c r="S4" s="25"/>
-    </row>
-    <row r="5" spans="1:19" ht="14.5" thickBot="1">
+      <c r="S4" s="58"/>
+    </row>
+    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="26"/>
       <c r="B5" s="29" t="s">
         <v>40</v>
@@ -2485,9 +2630,9 @@
       </c>
       <c r="J5" s="26"/>
       <c r="R5" s="27"/>
-      <c r="S5" s="25"/>
-    </row>
-    <row r="6" spans="1:19" ht="14.5" thickBot="1">
+      <c r="S5" s="58"/>
+    </row>
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33"/>
       <c r="B6" s="33" t="s">
         <v>46</v>
@@ -2515,387 +2660,515 @@
       </c>
       <c r="J6" s="36"/>
       <c r="R6" s="27"/>
-      <c r="S6" s="25"/>
-    </row>
-    <row r="7" spans="1:19">
+      <c r="S6" s="58"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="R7" s="27"/>
-      <c r="S7" s="25"/>
-    </row>
-    <row r="8" spans="1:19" ht="14" customHeight="1">
+      <c r="S7" s="58"/>
+    </row>
+    <row r="8" spans="1:19" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="93" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="98"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
+      <c r="C8" s="93"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="93"/>
+      <c r="F8" s="93"/>
       <c r="J8" s="38"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
-    </row>
-    <row r="9" spans="1:19">
+      <c r="R8" s="58"/>
+      <c r="S8" s="58"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="98" t="s">
+      <c r="B9" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="98"/>
-      <c r="D9" s="98"/>
-      <c r="E9" s="98"/>
-      <c r="F9" s="98"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="93"/>
+      <c r="E9" s="93"/>
+      <c r="F9" s="93"/>
       <c r="J9" s="39"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
-    </row>
-    <row r="10" spans="1:19">
+      <c r="R9" s="58"/>
+      <c r="S9" s="58"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="98" t="s">
+      <c r="B10" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="98"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="98"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="93"/>
       <c r="J10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-    </row>
-    <row r="11" spans="1:19">
+      <c r="R10" s="58"/>
+      <c r="S10" s="58"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="93" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="98"/>
-      <c r="D11" s="98"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="98"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-    </row>
-    <row r="12" spans="1:19">
+      <c r="C11" s="93"/>
+      <c r="D11" s="93"/>
+      <c r="E11" s="93"/>
+      <c r="F11" s="93"/>
+      <c r="R11" s="58"/>
+      <c r="S11" s="58"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="93" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="98"/>
-      <c r="D12" s="98"/>
-      <c r="E12" s="98"/>
-      <c r="F12" s="98"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-    </row>
-    <row r="14" spans="1:19" ht="14.5" thickBot="1">
+      <c r="C12" s="93"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="93"/>
+      <c r="R12" s="58"/>
+      <c r="S12" s="58"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" s="58"/>
+      <c r="B13" s="58"/>
+    </row>
+    <row r="14" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
       <c r="B14" s="27"/>
     </row>
-    <row r="15" spans="1:19" ht="28" thickBot="1">
-      <c r="A15" s="87" t="s">
+    <row r="15" spans="1:19" ht="28.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="80" t="s">
         <v>91</v>
       </c>
-      <c r="B15" s="88"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="88"/>
-      <c r="H15" s="88"/>
-      <c r="I15" s="89"/>
-    </row>
-    <row r="16" spans="1:19" ht="14.5" thickBot="1">
+      <c r="B15" s="81"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="82"/>
+      <c r="K15" s="80" t="s">
+        <v>92</v>
+      </c>
+      <c r="L15" s="81"/>
+      <c r="M15" s="81"/>
+      <c r="N15" s="81"/>
+      <c r="O15" s="81"/>
+      <c r="P15" s="82"/>
+    </row>
+    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>59</v>
       </c>
       <c r="B16" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="83" t="s">
+      <c r="C16" s="99" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="84"/>
-      <c r="E16" s="40" t="s">
+      <c r="D16" s="95"/>
+      <c r="E16" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="F16" s="83" t="s">
+      <c r="F16" s="99" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="84"/>
-      <c r="H16" s="85" t="s">
+      <c r="G16" s="95"/>
+      <c r="H16" s="94" t="s">
         <v>64</v>
       </c>
-      <c r="I16" s="84"/>
-    </row>
-    <row r="17" spans="1:10" ht="14.5" thickBot="1">
-      <c r="A17" s="26" t="s">
+      <c r="I16" s="95"/>
+      <c r="K16" s="99" t="s">
+        <v>61</v>
+      </c>
+      <c r="L16" s="95"/>
+      <c r="M16" s="94" t="s">
+        <v>93</v>
+      </c>
+      <c r="N16" s="94"/>
+      <c r="O16" s="111" t="s">
+        <v>94</v>
+      </c>
+      <c r="P16" s="112"/>
+    </row>
+    <row r="17" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="95" t="s">
+      <c r="C17" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="96"/>
-      <c r="E17" s="41" t="s">
+      <c r="D17" s="97"/>
+      <c r="E17" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="95" t="s">
+      <c r="F17" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="G17" s="96"/>
-      <c r="H17" s="97" t="s">
+      <c r="G17" s="97"/>
+      <c r="H17" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="I17" s="96"/>
-    </row>
-    <row r="18" spans="1:10" ht="14" customHeight="1">
-      <c r="A18" s="93" t="s">
+      <c r="I17" s="97"/>
+      <c r="K17" s="109" t="s">
+        <v>65</v>
+      </c>
+      <c r="L17" s="110"/>
+      <c r="M17" s="101" t="s">
+        <v>66</v>
+      </c>
+      <c r="N17" s="101"/>
+      <c r="O17" s="113" t="s">
+        <v>95</v>
+      </c>
+      <c r="P17" s="114"/>
+    </row>
+    <row r="18" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="107" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="94"/>
-      <c r="C18" s="42" t="s">
+      <c r="B18" s="108"/>
+      <c r="C18" s="40" t="s">
         <v>70</v>
       </c>
-      <c r="D18" s="43"/>
-      <c r="E18" s="90" t="s">
+      <c r="D18" s="60"/>
+      <c r="E18" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="F18" s="82" t="s">
+      <c r="F18" s="100" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="82"/>
-      <c r="H18" s="122" t="s">
+      <c r="G18" s="100"/>
+      <c r="H18" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="I18" s="123" t="s">
+      <c r="I18" s="68" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="78" t="s">
+      <c r="K18" s="116" t="s">
+        <v>96</v>
+      </c>
+      <c r="L18" s="100"/>
+      <c r="M18" s="116" t="s">
+        <v>98</v>
+      </c>
+      <c r="N18" s="117"/>
+      <c r="O18" s="121" t="s">
+        <v>99</v>
+      </c>
+      <c r="P18" s="122"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="109" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="75"/>
-      <c r="C19" s="44" t="s">
+      <c r="B19" s="110"/>
+      <c r="C19" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="45"/>
-      <c r="E19" s="91"/>
-      <c r="F19" s="44" t="s">
+      <c r="D19" s="59"/>
+      <c r="E19" s="103"/>
+      <c r="F19" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="G19" s="25" t="s">
+      <c r="G19" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="H19" s="44" t="s">
+      <c r="H19" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="I19" s="45" t="s">
+      <c r="I19" s="59" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="78" t="s">
+      <c r="K19" s="109" t="s">
+        <v>71</v>
+      </c>
+      <c r="L19" s="101"/>
+      <c r="M19" s="109"/>
+      <c r="N19" s="110"/>
+      <c r="O19" s="115" t="s">
+        <v>103</v>
+      </c>
+      <c r="P19" s="114"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="109" t="s">
         <v>69</v>
       </c>
-      <c r="B20" s="75"/>
-      <c r="C20" s="44" t="s">
+      <c r="B20" s="110"/>
+      <c r="C20" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="45"/>
-      <c r="E20" s="91"/>
-      <c r="F20" s="74" t="s">
+      <c r="D20" s="59"/>
+      <c r="E20" s="103"/>
+      <c r="F20" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="G20" s="74"/>
-      <c r="H20" s="44" t="s">
+      <c r="G20" s="101"/>
+      <c r="H20" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="I20" s="45" t="s">
+      <c r="I20" s="59" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="78" t="s">
+      <c r="K20" s="109" t="s">
+        <v>97</v>
+      </c>
+      <c r="L20" s="101"/>
+      <c r="M20" s="109"/>
+      <c r="N20" s="110"/>
+      <c r="O20" s="115" t="s">
+        <v>100</v>
+      </c>
+      <c r="P20" s="114"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="109" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="75"/>
-      <c r="C21" s="46" t="s">
+      <c r="B21" s="110"/>
+      <c r="C21" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="D21" s="47"/>
-      <c r="E21" s="91"/>
-      <c r="F21" s="44" t="s">
+      <c r="D21" s="43"/>
+      <c r="E21" s="103"/>
+      <c r="F21" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="G21" s="25" t="s">
+      <c r="G21" s="58" t="s">
         <v>80</v>
       </c>
-      <c r="H21" s="44" t="s">
+      <c r="H21" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="I21" s="121" t="s">
+      <c r="I21" s="66" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="14.5" thickBot="1">
-      <c r="A22" s="79" t="s">
+      <c r="K21" s="109"/>
+      <c r="L21" s="101"/>
+      <c r="M21" s="109"/>
+      <c r="N21" s="110"/>
+      <c r="O21" s="115" t="s">
+        <v>101</v>
+      </c>
+      <c r="P21" s="114"/>
+    </row>
+    <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="105" t="s">
         <v>90</v>
       </c>
-      <c r="B22" s="80"/>
-      <c r="C22" s="48"/>
-      <c r="D22" s="41" t="s">
+      <c r="B22" s="106"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="E22" s="92"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="48" t="s">
+      <c r="E22" s="104"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="I22" s="49"/>
-    </row>
-    <row r="24" spans="1:10" ht="14.5" thickBot="1"/>
-    <row r="25" spans="1:10" ht="28" thickBot="1">
-      <c r="A25" s="109" t="s">
-        <v>92</v>
-      </c>
-      <c r="B25" s="110"/>
-      <c r="C25" s="110"/>
-      <c r="D25" s="110"/>
-      <c r="E25" s="110"/>
-      <c r="F25" s="111"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-    </row>
-    <row r="26" spans="1:10" ht="14.5" thickBot="1">
-      <c r="A26" s="83" t="s">
+      <c r="I22" s="61"/>
+      <c r="K22" s="105"/>
+      <c r="L22" s="118"/>
+      <c r="M22" s="105"/>
+      <c r="N22" s="106"/>
+      <c r="O22" s="119" t="s">
+        <v>102</v>
+      </c>
+      <c r="P22" s="120"/>
+    </row>
+    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:16" ht="28.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="80" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="81"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="81"/>
+      <c r="G24" s="81"/>
+      <c r="H24" s="81"/>
+      <c r="I24" s="82"/>
+      <c r="J24" s="38"/>
+    </row>
+    <row r="25" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="99" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="84"/>
-      <c r="C26" s="85" t="s">
-        <v>93</v>
-      </c>
-      <c r="D26" s="85"/>
-      <c r="E26" s="112" t="s">
-        <v>94</v>
-      </c>
-      <c r="F26" s="113"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="86"/>
-      <c r="J26" s="86"/>
-    </row>
-    <row r="27" spans="1:10" ht="14.5" thickBot="1">
-      <c r="A27" s="78" t="s">
+      <c r="D25" s="95"/>
+      <c r="E25" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="F25" s="99" t="s">
+        <v>116</v>
+      </c>
+      <c r="G25" s="95"/>
+      <c r="H25" s="94" t="s">
+        <v>116</v>
+      </c>
+      <c r="I25" s="95"/>
+      <c r="J25" s="64"/>
+    </row>
+    <row r="26" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="96" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="75"/>
-      <c r="C27" s="74" t="s">
+      <c r="D26" s="97"/>
+      <c r="E26" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="74"/>
-      <c r="E27" s="114" t="s">
-        <v>95</v>
-      </c>
-      <c r="F27" s="115"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="74"/>
-      <c r="J27" s="74"/>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="76" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="82"/>
-      <c r="C28" s="76" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28" s="77"/>
-      <c r="E28" s="116" t="s">
-        <v>99</v>
-      </c>
-      <c r="F28" s="117"/>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="74"/>
-      <c r="C29" s="78"/>
-      <c r="D29" s="75"/>
-      <c r="E29" s="118" t="s">
-        <v>103</v>
-      </c>
-      <c r="F29" s="115"/>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="78" t="s">
-        <v>97</v>
-      </c>
-      <c r="B30" s="74"/>
-      <c r="C30" s="78"/>
-      <c r="D30" s="75"/>
-      <c r="E30" s="118" t="s">
-        <v>100</v>
-      </c>
-      <c r="F30" s="115"/>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="78"/>
-      <c r="B31" s="74"/>
-      <c r="C31" s="78"/>
-      <c r="D31" s="75"/>
-      <c r="E31" s="118" t="s">
-        <v>101</v>
-      </c>
-      <c r="F31" s="115"/>
-    </row>
-    <row r="32" spans="1:10" ht="14.5" thickBot="1">
-      <c r="A32" s="79"/>
-      <c r="B32" s="81"/>
-      <c r="C32" s="79"/>
-      <c r="D32" s="80"/>
-      <c r="E32" s="119" t="s">
-        <v>102</v>
-      </c>
-      <c r="F32" s="120"/>
+      <c r="G26" s="97"/>
+      <c r="H26" s="98" t="s">
+        <v>65</v>
+      </c>
+      <c r="I26" s="97"/>
+      <c r="J26" s="58"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" s="127" t="s">
+        <v>115</v>
+      </c>
+      <c r="B27" s="128" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="116" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="100"/>
+      <c r="E27" s="102" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="116" t="s">
+        <v>114</v>
+      </c>
+      <c r="G27" s="117"/>
+      <c r="H27" s="131" t="s">
+        <v>114</v>
+      </c>
+      <c r="I27" s="132"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A28" s="129" t="s">
+        <v>115</v>
+      </c>
+      <c r="B28" s="130"/>
+      <c r="C28" s="109" t="s">
+        <v>113</v>
+      </c>
+      <c r="D28" s="101"/>
+      <c r="E28" s="103"/>
+      <c r="F28" s="109"/>
+      <c r="G28" s="110"/>
+      <c r="H28" s="133"/>
+      <c r="I28" s="134"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A29" s="109"/>
+      <c r="B29" s="110"/>
+      <c r="C29" s="109" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="101"/>
+      <c r="E29" s="103"/>
+      <c r="F29" s="109"/>
+      <c r="G29" s="110"/>
+      <c r="H29" s="133"/>
+      <c r="I29" s="134"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A30" s="109"/>
+      <c r="B30" s="110"/>
+      <c r="C30" s="123" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="125"/>
+      <c r="E30" s="103"/>
+      <c r="F30" s="109"/>
+      <c r="G30" s="110"/>
+      <c r="H30" s="133"/>
+      <c r="I30" s="134"/>
+    </row>
+    <row r="31" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="105"/>
+      <c r="B31" s="106"/>
+      <c r="C31" s="124" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="126"/>
+      <c r="E31" s="104"/>
+      <c r="F31" s="105"/>
+      <c r="G31" s="106"/>
+      <c r="H31" s="135"/>
+      <c r="I31" s="136"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="F16:G16"/>
+  <mergeCells count="61">
+    <mergeCell ref="K15:P15"/>
+    <mergeCell ref="E27:E31"/>
+    <mergeCell ref="F27:G31"/>
+    <mergeCell ref="H27:I31"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="A28:B31"/>
+    <mergeCell ref="A24:I24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="M18:N22"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="O20:P20"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="F20:G20"/>
     <mergeCell ref="E18:E22"/>
@@ -2904,28 +3177,31 @@
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C28:D32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="B27 E27:F27 H27" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>